<commit_message>
Entries for Endeavour, Black Pear, OMS
</commit_message>
<xml_diff>
--- a/transform-register.xlsx
+++ b/transform-register.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10319"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ian/Dropbox/Development/inidus/github/Transform-registry/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{476A973E-5A20-F14C-BCBD-8C8E7FC06C3D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8260" yWindow="2200" windowWidth="37660" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8265" yWindow="2205" windowWidth="37665" windowHeight="18855"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="45">
   <si>
     <t>Status</t>
   </si>
@@ -82,13 +76,88 @@
   </si>
   <si>
     <t>Based on early draft of  Care-Connect STU3 - will be updated when that is published</t>
+  </si>
+  <si>
+    <t>david.stables@endeavourhealth.org</t>
+  </si>
+  <si>
+    <t>FHIR - most main resources</t>
+  </si>
+  <si>
+    <t>Emis Proprietary csv format</t>
+  </si>
+  <si>
+    <t>TPP proprietary csv format</t>
+  </si>
+  <si>
+    <t>HL7 V2 ADT (Barts Patient admission &amp; discharge)</t>
+  </si>
+  <si>
+    <t>HL7 V2 ADT (Homerton Patient admission &amp; discharge)</t>
+  </si>
+  <si>
+    <t>Cerner Millenium Patients, diagnoses, procedures (Barts)</t>
+  </si>
+  <si>
+    <t>FHIR - Patient, Encounter, care episode</t>
+  </si>
+  <si>
+    <t>FHIR - patient, encounter, observation, condition, care episode</t>
+  </si>
+  <si>
+    <t>Cerner Millenium clinical events (Barts)</t>
+  </si>
+  <si>
+    <t>Adastra - case closure proprietary XML</t>
+  </si>
+  <si>
+    <t>currently FHIR STU2 older version (CareConnect?)</t>
+  </si>
+  <si>
+    <t>complete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dunmail@blackpear.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/HL7-UK/Transform-registry/BlackPear </t>
+  </si>
+  <si>
+    <t>test cases for 4 query responses available</t>
+  </si>
+  <si>
+    <t>FHIR OperationOutcome, Patient, Organization</t>
+  </si>
+  <si>
+    <t>Vision proprietary csv format</t>
+  </si>
+  <si>
+    <t>NHS Spine  - PDS SMSP query responses</t>
+  </si>
+  <si>
+    <t>https://github.com/endeavourhealth/Transforms</t>
+  </si>
+  <si>
+    <t>HL7 V2 ADT</t>
+  </si>
+  <si>
+    <t>FHIR Patient Practitioner</t>
+  </si>
+  <si>
+    <t>rpworden@me.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/HL7-UK/Transform-registry/OMS </t>
+  </si>
+  <si>
+    <t>Java transform generated using Transform By Example (TBE) tools. Uses HAPI libraries. Inverse transform available</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,7 +291,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -254,27 +323,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -306,24 +357,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -499,26 +532,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.5" style="2" customWidth="1"/>
+    <col min="1" max="1" width="36.5703125" style="2" customWidth="1"/>
     <col min="2" max="2" width="37" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" customWidth="1"/>
-    <col min="4" max="4" width="29.33203125" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" customWidth="1"/>
-    <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="58.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="37.28515625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="35" style="5" customWidth="1"/>
+    <col min="8" max="8" width="58.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -534,7 +567,7 @@
       <c r="E1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="3" t="s">
@@ -544,7 +577,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="45">
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
@@ -560,7 +593,7 @@
       <c r="E2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>18</v>
       </c>
       <c r="G2" s="9" t="s">
@@ -570,7 +603,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="45">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
@@ -586,7 +619,7 @@
       <c r="E3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>18</v>
       </c>
       <c r="G3" s="5" t="s">
@@ -596,7 +629,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="45">
       <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
@@ -612,7 +645,7 @@
       <c r="E4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>18</v>
       </c>
       <c r="G4" s="5" t="s">
@@ -622,7 +655,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="45">
       <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
@@ -638,7 +671,7 @@
       <c r="E5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>18</v>
       </c>
       <c r="G5" s="5" t="s">
@@ -648,138 +681,353 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
+    <row r="6" spans="1:8" ht="30">
+      <c r="A6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="8">
+        <v>43210</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="30">
+      <c r="A7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="8">
+        <v>43210</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30">
+      <c r="A8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="8">
+        <v>43210</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="30">
+      <c r="A9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="8">
+        <v>43210</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30">
+      <c r="A10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="8">
+        <v>43210</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30">
+      <c r="A11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="8">
+        <v>43210</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30">
+      <c r="A12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="8">
+        <v>43210</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30">
+      <c r="A13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="8">
+        <v>43210</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="30">
+      <c r="A14" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="8">
+        <v>43245</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="30">
+      <c r="A15" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="8">
+        <v>43251</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="30">
+      <c r="A16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="8">
+        <v>43251</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{112D821E-3B9D-2A46-905D-0AB734505EA1}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{341FE4C0-8D27-8045-8FBF-0D6BB83471AB}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{FBB5E8C1-5DC0-FF48-B073-64560BD145DF}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{E6CD624A-DF4E-D14C-99B4-D98608C13974}"/>
-    <hyperlink ref="G2" r:id="rId5" xr:uid="{A6BC88A6-59B2-0A41-9D3D-B3DA9BFA707B}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="G2" r:id="rId5"/>
+    <hyperlink ref="D6" r:id="rId6"/>
+    <hyperlink ref="D7" r:id="rId7"/>
+    <hyperlink ref="D8" r:id="rId8"/>
+    <hyperlink ref="D9" r:id="rId9"/>
+    <hyperlink ref="D10" r:id="rId10"/>
+    <hyperlink ref="D11" r:id="rId11"/>
+    <hyperlink ref="D12" r:id="rId12"/>
+    <hyperlink ref="D13" r:id="rId13"/>
+    <hyperlink ref="D14" r:id="rId14"/>
+    <hyperlink ref="F14" r:id="rId15"/>
+    <hyperlink ref="F6" r:id="rId16"/>
+    <hyperlink ref="G6" r:id="rId17"/>
+    <hyperlink ref="F7" r:id="rId18"/>
+    <hyperlink ref="F8" r:id="rId19"/>
+    <hyperlink ref="F9" r:id="rId20"/>
+    <hyperlink ref="F10" r:id="rId21"/>
+    <hyperlink ref="F11" r:id="rId22"/>
+    <hyperlink ref="F12" r:id="rId23"/>
+    <hyperlink ref="F13" r:id="rId24"/>
+    <hyperlink ref="G7" r:id="rId25"/>
+    <hyperlink ref="G8" r:id="rId26"/>
+    <hyperlink ref="G9" r:id="rId27"/>
+    <hyperlink ref="G10" r:id="rId28"/>
+    <hyperlink ref="G11" r:id="rId29"/>
+    <hyperlink ref="G12" r:id="rId30"/>
+    <hyperlink ref="G13" r:id="rId31"/>
+    <hyperlink ref="D15" r:id="rId32"/>
+    <hyperlink ref="D16" r:id="rId33"/>
+    <hyperlink ref="F15" r:id="rId34"/>
+    <hyperlink ref="G15" r:id="rId35"/>
+    <hyperlink ref="F16" r:id="rId36"/>
+    <hyperlink ref="G16" r:id="rId37"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId38"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>